<commit_message>
3 days expense added
</commit_message>
<xml_diff>
--- a/ExpenseTracker_Template.xlsx
+++ b/ExpenseTracker_Template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amlan.patra\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nucleusonline-my.sharepoint.com/personal/amlan_patra_nucleussoftware_com/Documents/Desktop/excel-expense-track/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36D53DAF-A4E2-44AE-AC85-44193FFB47E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{36D53DAF-A4E2-44AE-AC85-44193FFB47E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{70DB20C2-293D-46E8-BAB6-D87B302D4072}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -96,13 +96,13 @@
     <t>SBI</t>
   </si>
   <si>
-    <t xml:space="preserve">Adding Up ? </t>
-  </si>
-  <si>
     <t xml:space="preserve">Note : </t>
   </si>
   <si>
     <t>Current Daily avg expense is only valid for current month</t>
+  </si>
+  <si>
+    <t>Mb expense</t>
   </si>
 </sst>
 </file>
@@ -307,13 +307,13 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -549,7 +549,7 @@
   <dimension ref="A1:G1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -565,13 +565,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="20.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
@@ -608,8 +608,8 @@
         <v>30000</v>
       </c>
       <c r="D3" s="3">
-        <f ca="1">ROUND(C3/(DAY(EOMONTH(Expenses!$A2,0))),2)</f>
-        <v>1000</v>
+        <f>ROUND(C3/(DAY(EOMONTH(Expenses!$A2,0))),2)</f>
+        <v>967.74</v>
       </c>
       <c r="E3" s="3">
         <f>C3-G3</f>
@@ -617,7 +617,7 @@
       </c>
       <c r="F3" s="3">
         <f ca="1" xml:space="preserve"> ROUND(E3/(IF( (DATEDIF(TODAY(),EOMONTH(TODAY(),0),"D")) &gt; 0, (DATEDIF(TODAY(),EOMONTH(TODAY(),0),"D")), 1)),2)</f>
-        <v>30000</v>
+        <v>1000</v>
       </c>
       <c r="G3" s="3">
         <f>SUM(Expenses!B2:B31)</f>
@@ -637,9 +637,9 @@
       <c r="A6" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="15">
-        <f>DATE(2023,11,1)</f>
-        <v>45231</v>
+      <c r="B6" s="13">
+        <f>DATE(2023,12,1)</f>
+        <v>45261</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15" customHeight="1">
@@ -648,18 +648,18 @@
       </c>
       <c r="B8">
         <f>DAY(EOMONTH(B6,0))</f>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15" customHeight="1">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
     </row>
     <row r="21" spans="1:4" ht="15.75" customHeight="1"/>
     <row r="22" spans="1:4" ht="15.75" customHeight="1"/>
@@ -1656,19 +1656,21 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J34" sqref="J34"/>
+      <selection pane="bottomLeft" activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="11.28515625" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
     <col min="3" max="3" width="10.28515625" customWidth="1"/>
     <col min="4" max="4" width="8.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1"/>
     <col min="6" max="6" width="9.140625" customWidth="1"/>
     <col min="7" max="7" width="6.5703125" customWidth="1"/>
     <col min="8" max="8" width="7" customWidth="1"/>
     <col min="9" max="9" width="6.140625" customWidth="1"/>
-    <col min="10" max="10" width="25" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="25.5">
@@ -1700,7 +1702,7 @@
         <v>18</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
@@ -1721,19 +1723,20 @@
     </row>
     <row r="2" spans="1:26">
       <c r="A2" s="7">
-        <f ca="1">EOMONTH(TODAY(),-1)+1</f>
-        <v>45231</v>
+        <f>Info!B6</f>
+        <v>45261</v>
       </c>
       <c r="B2" s="8">
+        <f>F2+G2+H2+I2+J2</f>
         <v>0</v>
       </c>
       <c r="C2" s="9">
-        <f ca="1">Info!D3-B2</f>
-        <v>1000</v>
+        <f>Info!D3-B2</f>
+        <v>967.74</v>
       </c>
       <c r="D2" s="10">
-        <f ca="1">C2</f>
-        <v>1000</v>
+        <f>C2</f>
+        <v>967.74</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -1760,19 +1763,20 @@
     </row>
     <row r="3" spans="1:26">
       <c r="A3" s="7">
-        <f ca="1">EOMONTH(TODAY(),-1)+2</f>
-        <v>45232</v>
+        <f>A2+1</f>
+        <v>45262</v>
       </c>
       <c r="B3" s="8">
+        <f>F3+G3+H3+I3+J3</f>
         <v>0</v>
       </c>
       <c r="C3" s="9">
-        <f ca="1">Info!D3-B3</f>
-        <v>1000</v>
+        <f>Info!D3-B3</f>
+        <v>967.74</v>
       </c>
       <c r="D3" s="10">
-        <f t="shared" ref="D3:D31" ca="1" si="0">D2+C3</f>
-        <v>2000</v>
+        <f t="shared" ref="D3:D31" si="0">D2+C3</f>
+        <v>1935.48</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="11"/>
@@ -1799,19 +1803,20 @@
     </row>
     <row r="4" spans="1:26">
       <c r="A4" s="7">
-        <f ca="1">EOMONTH(TODAY(),-1)+3</f>
-        <v>45233</v>
+        <f>A3+1</f>
+        <v>45263</v>
       </c>
       <c r="B4" s="8">
+        <f t="shared" ref="B4:B32" si="1">F4+G4+H4+I4+J4</f>
         <v>0</v>
       </c>
       <c r="C4" s="9">
-        <f ca="1">Info!D3-B4</f>
-        <v>1000</v>
+        <f>Info!D3-B4</f>
+        <v>967.74</v>
       </c>
       <c r="D4" s="10">
-        <f t="shared" ca="1" si="0"/>
-        <v>3000</v>
+        <f t="shared" si="0"/>
+        <v>2903.2200000000003</v>
       </c>
       <c r="E4" s="8"/>
       <c r="F4" s="4"/>
@@ -1838,19 +1843,20 @@
     </row>
     <row r="5" spans="1:26">
       <c r="A5" s="7">
-        <f ca="1">EOMONTH(TODAY(),-1)+4</f>
-        <v>45234</v>
+        <f t="shared" ref="A5:A32" si="2">A4+1</f>
+        <v>45264</v>
       </c>
       <c r="B5" s="8">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C5" s="9">
-        <f ca="1">Info!D3-B5</f>
-        <v>1000</v>
+        <f>Info!D3-B5</f>
+        <v>967.74</v>
       </c>
       <c r="D5" s="10">
-        <f t="shared" ca="1" si="0"/>
-        <v>4000</v>
+        <f t="shared" si="0"/>
+        <v>3870.96</v>
       </c>
       <c r="E5" s="8"/>
       <c r="F5" s="4"/>
@@ -1877,19 +1883,20 @@
     </row>
     <row r="6" spans="1:26">
       <c r="A6" s="7">
-        <f ca="1">EOMONTH(TODAY(),-1)+5</f>
-        <v>45235</v>
+        <f t="shared" si="2"/>
+        <v>45265</v>
       </c>
       <c r="B6" s="8">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C6" s="9">
-        <f ca="1">Info!D3-B6</f>
-        <v>1000</v>
+        <f>Info!D3-B6</f>
+        <v>967.74</v>
       </c>
       <c r="D6" s="10">
-        <f t="shared" ca="1" si="0"/>
-        <v>5000</v>
+        <f t="shared" si="0"/>
+        <v>4838.7</v>
       </c>
       <c r="E6" s="8"/>
       <c r="F6" s="4"/>
@@ -1916,19 +1923,20 @@
     </row>
     <row r="7" spans="1:26">
       <c r="A7" s="7">
-        <f ca="1">EOMONTH(TODAY(),-1)+6</f>
-        <v>45236</v>
+        <f t="shared" si="2"/>
+        <v>45266</v>
       </c>
       <c r="B7" s="8">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C7" s="9">
-        <f ca="1">Info!D3-B7</f>
-        <v>1000</v>
+        <f>Info!D3-B7</f>
+        <v>967.74</v>
       </c>
       <c r="D7" s="10">
-        <f t="shared" ca="1" si="0"/>
-        <v>6000</v>
+        <f t="shared" si="0"/>
+        <v>5806.44</v>
       </c>
       <c r="E7" s="8"/>
       <c r="F7" s="4"/>
@@ -1955,19 +1963,20 @@
     </row>
     <row r="8" spans="1:26">
       <c r="A8" s="7">
-        <f ca="1">EOMONTH(TODAY(),-1)+7</f>
-        <v>45237</v>
+        <f t="shared" si="2"/>
+        <v>45267</v>
       </c>
       <c r="B8" s="8">
+        <f>F8+G8+H8+I8+J8</f>
         <v>0</v>
       </c>
       <c r="C8" s="9">
-        <f ca="1">Info!D3-B8</f>
-        <v>1000</v>
+        <f>Info!D3-B8</f>
+        <v>967.74</v>
       </c>
       <c r="D8" s="10">
-        <f t="shared" ca="1" si="0"/>
-        <v>7000</v>
+        <f t="shared" si="0"/>
+        <v>6774.1799999999994</v>
       </c>
       <c r="E8" s="8"/>
       <c r="F8" s="4"/>
@@ -1994,19 +2003,20 @@
     </row>
     <row r="9" spans="1:26">
       <c r="A9" s="7">
-        <f ca="1">EOMONTH(TODAY(),-1)+8</f>
-        <v>45238</v>
+        <f t="shared" si="2"/>
+        <v>45268</v>
       </c>
       <c r="B9" s="8">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C9" s="9">
-        <f ca="1">Info!D3-B9</f>
-        <v>1000</v>
+        <f>Info!D3-B9</f>
+        <v>967.74</v>
       </c>
       <c r="D9" s="10">
-        <f t="shared" ca="1" si="0"/>
-        <v>8000</v>
+        <f t="shared" si="0"/>
+        <v>7741.9199999999992</v>
       </c>
       <c r="E9" s="8"/>
       <c r="F9" s="4"/>
@@ -2033,19 +2043,20 @@
     </row>
     <row r="10" spans="1:26">
       <c r="A10" s="7">
-        <f ca="1">EOMONTH(TODAY(),-1)+9</f>
-        <v>45239</v>
+        <f t="shared" si="2"/>
+        <v>45269</v>
       </c>
       <c r="B10" s="8">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C10" s="9">
-        <f ca="1">Info!D3-B10</f>
-        <v>1000</v>
+        <f>Info!D3-B10</f>
+        <v>967.74</v>
       </c>
       <c r="D10" s="10">
-        <f t="shared" ca="1" si="0"/>
-        <v>9000</v>
+        <f t="shared" si="0"/>
+        <v>8709.66</v>
       </c>
       <c r="E10" s="12"/>
       <c r="F10" s="4"/>
@@ -2072,19 +2083,20 @@
     </row>
     <row r="11" spans="1:26">
       <c r="A11" s="7">
-        <f ca="1">EOMONTH(TODAY(),-1)+10</f>
-        <v>45240</v>
+        <f t="shared" si="2"/>
+        <v>45270</v>
       </c>
       <c r="B11" s="8">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C11" s="9">
-        <f ca="1">Info!D3-B11</f>
-        <v>1000</v>
+        <f>Info!D3-B11</f>
+        <v>967.74</v>
       </c>
       <c r="D11" s="10">
-        <f t="shared" ca="1" si="0"/>
-        <v>10000</v>
+        <f t="shared" si="0"/>
+        <v>9677.4</v>
       </c>
       <c r="E11" s="8"/>
       <c r="F11" s="4"/>
@@ -2111,19 +2123,20 @@
     </row>
     <row r="12" spans="1:26">
       <c r="A12" s="7">
-        <f ca="1">EOMONTH(TODAY(),-1)+11</f>
-        <v>45241</v>
+        <f t="shared" si="2"/>
+        <v>45271</v>
       </c>
       <c r="B12" s="8">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C12" s="9">
-        <f ca="1">Info!D3-B12</f>
-        <v>1000</v>
+        <f>Info!D3-B12</f>
+        <v>967.74</v>
       </c>
       <c r="D12" s="10">
-        <f t="shared" ca="1" si="0"/>
-        <v>11000</v>
+        <f t="shared" si="0"/>
+        <v>10645.14</v>
       </c>
       <c r="E12" s="8"/>
       <c r="F12" s="4"/>
@@ -2150,19 +2163,20 @@
     </row>
     <row r="13" spans="1:26">
       <c r="A13" s="7">
-        <f ca="1">EOMONTH(TODAY(),-1)+12</f>
-        <v>45242</v>
+        <f t="shared" si="2"/>
+        <v>45272</v>
       </c>
       <c r="B13" s="8">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C13" s="9">
-        <f ca="1">Info!D3-B13</f>
-        <v>1000</v>
+        <f>Info!D3-B13</f>
+        <v>967.74</v>
       </c>
       <c r="D13" s="10">
-        <f t="shared" ca="1" si="0"/>
-        <v>12000</v>
+        <f t="shared" si="0"/>
+        <v>11612.88</v>
       </c>
       <c r="E13" s="8"/>
       <c r="F13" s="4"/>
@@ -2189,19 +2203,20 @@
     </row>
     <row r="14" spans="1:26">
       <c r="A14" s="7">
-        <f ca="1">EOMONTH(TODAY(),-1)+13</f>
-        <v>45243</v>
+        <f t="shared" si="2"/>
+        <v>45273</v>
       </c>
       <c r="B14" s="8">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C14" s="9">
-        <f ca="1">Info!D3-B14</f>
-        <v>1000</v>
+        <f>Info!D3-B14</f>
+        <v>967.74</v>
       </c>
       <c r="D14" s="10">
-        <f t="shared" ca="1" si="0"/>
-        <v>13000</v>
+        <f t="shared" si="0"/>
+        <v>12580.619999999999</v>
       </c>
       <c r="E14" s="8"/>
       <c r="F14" s="4"/>
@@ -2228,19 +2243,20 @@
     </row>
     <row r="15" spans="1:26">
       <c r="A15" s="7">
-        <f ca="1">EOMONTH(TODAY(),-1)+14</f>
-        <v>45244</v>
+        <f t="shared" si="2"/>
+        <v>45274</v>
       </c>
       <c r="B15" s="8">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C15" s="9">
-        <f ca="1">Info!D3-B15</f>
-        <v>1000</v>
+        <f>Info!D3-B15</f>
+        <v>967.74</v>
       </c>
       <c r="D15" s="10">
-        <f t="shared" ca="1" si="0"/>
-        <v>14000</v>
+        <f t="shared" si="0"/>
+        <v>13548.359999999999</v>
       </c>
       <c r="E15" s="8"/>
       <c r="F15" s="4"/>
@@ -2267,19 +2283,20 @@
     </row>
     <row r="16" spans="1:26">
       <c r="A16" s="7">
-        <f ca="1">EOMONTH(TODAY(),-1)+15</f>
-        <v>45245</v>
+        <f t="shared" si="2"/>
+        <v>45275</v>
       </c>
       <c r="B16" s="8">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C16" s="9">
-        <f ca="1">Info!D3-B16</f>
-        <v>1000</v>
+        <f>Info!D3-B16</f>
+        <v>967.74</v>
       </c>
       <c r="D16" s="10">
-        <f t="shared" ca="1" si="0"/>
-        <v>15000</v>
+        <f t="shared" si="0"/>
+        <v>14516.099999999999</v>
       </c>
       <c r="E16" s="8"/>
       <c r="F16" s="4"/>
@@ -2305,19 +2322,20 @@
     </row>
     <row r="17" spans="1:26">
       <c r="A17" s="7">
-        <f ca="1">EOMONTH(TODAY(),-1)+16</f>
-        <v>45246</v>
+        <f t="shared" si="2"/>
+        <v>45276</v>
       </c>
       <c r="B17" s="8">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C17" s="9">
-        <f ca="1">Info!D3-B17</f>
-        <v>1000</v>
+        <f>Info!D3-B17</f>
+        <v>967.74</v>
       </c>
       <c r="D17" s="10">
-        <f t="shared" ca="1" si="0"/>
-        <v>16000</v>
+        <f t="shared" si="0"/>
+        <v>15483.839999999998</v>
       </c>
       <c r="E17" s="8"/>
       <c r="F17" s="4"/>
@@ -2343,19 +2361,20 @@
     </row>
     <row r="18" spans="1:26">
       <c r="A18" s="7">
-        <f ca="1">EOMONTH(TODAY(),-1)+17</f>
-        <v>45247</v>
+        <f t="shared" si="2"/>
+        <v>45277</v>
       </c>
       <c r="B18" s="8">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C18" s="9">
-        <f ca="1">Info!D3-B18</f>
-        <v>1000</v>
+        <f>Info!D3-B18</f>
+        <v>967.74</v>
       </c>
       <c r="D18" s="10">
-        <f t="shared" ca="1" si="0"/>
-        <v>17000</v>
+        <f t="shared" si="0"/>
+        <v>16451.579999999998</v>
       </c>
       <c r="E18" s="8"/>
       <c r="F18" s="4"/>
@@ -2381,19 +2400,20 @@
     </row>
     <row r="19" spans="1:26">
       <c r="A19" s="7">
-        <f ca="1">EOMONTH(TODAY(),-1)+18</f>
-        <v>45248</v>
+        <f t="shared" si="2"/>
+        <v>45278</v>
       </c>
       <c r="B19" s="8">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C19" s="9">
-        <f ca="1">Info!D3-B19</f>
-        <v>1000</v>
+        <f>Info!D3-B19</f>
+        <v>967.74</v>
       </c>
       <c r="D19" s="10">
-        <f t="shared" ca="1" si="0"/>
-        <v>18000</v>
+        <f t="shared" si="0"/>
+        <v>17419.32</v>
       </c>
       <c r="E19" s="8"/>
       <c r="F19" s="4"/>
@@ -2420,19 +2440,20 @@
     </row>
     <row r="20" spans="1:26">
       <c r="A20" s="7">
-        <f ca="1">EOMONTH(TODAY(),-1)+19</f>
-        <v>45249</v>
+        <f t="shared" si="2"/>
+        <v>45279</v>
       </c>
       <c r="B20" s="8">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C20" s="9">
-        <f ca="1">Info!D3-B20</f>
-        <v>1000</v>
+        <f>Info!D3-B20</f>
+        <v>967.74</v>
       </c>
       <c r="D20" s="10">
-        <f t="shared" ca="1" si="0"/>
-        <v>19000</v>
+        <f t="shared" si="0"/>
+        <v>18387.060000000001</v>
       </c>
       <c r="E20" s="8"/>
       <c r="F20" s="4"/>
@@ -2459,19 +2480,20 @@
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1">
       <c r="A21" s="7">
-        <f ca="1">EOMONTH(TODAY(),-1)+20</f>
-        <v>45250</v>
+        <f t="shared" si="2"/>
+        <v>45280</v>
       </c>
       <c r="B21" s="8">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C21" s="9">
-        <f ca="1">Info!D3-B21</f>
-        <v>1000</v>
+        <f>Info!D3-B21</f>
+        <v>967.74</v>
       </c>
       <c r="D21" s="10">
-        <f t="shared" ca="1" si="0"/>
-        <v>20000</v>
+        <f t="shared" si="0"/>
+        <v>19354.800000000003</v>
       </c>
       <c r="E21" s="8"/>
       <c r="F21" s="4"/>
@@ -2498,19 +2520,20 @@
     </row>
     <row r="22" spans="1:26" ht="15.75" customHeight="1">
       <c r="A22" s="7">
-        <f ca="1">EOMONTH(TODAY(),-1)+21</f>
-        <v>45251</v>
+        <f t="shared" si="2"/>
+        <v>45281</v>
       </c>
       <c r="B22" s="8">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C22" s="9">
-        <f ca="1">Info!D3-B22</f>
-        <v>1000</v>
+        <f>Info!D3-B22</f>
+        <v>967.74</v>
       </c>
       <c r="D22" s="10">
-        <f t="shared" ca="1" si="0"/>
-        <v>21000</v>
+        <f t="shared" si="0"/>
+        <v>20322.540000000005</v>
       </c>
       <c r="E22" s="8"/>
       <c r="F22" s="4"/>
@@ -2537,19 +2560,20 @@
     </row>
     <row r="23" spans="1:26" ht="15.75" customHeight="1">
       <c r="A23" s="7">
-        <f ca="1">EOMONTH(TODAY(),-1)+22</f>
-        <v>45252</v>
+        <f t="shared" si="2"/>
+        <v>45282</v>
       </c>
       <c r="B23" s="8">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C23" s="9">
-        <f ca="1">Info!D3-B23</f>
-        <v>1000</v>
+        <f>Info!D3-B23</f>
+        <v>967.74</v>
       </c>
       <c r="D23" s="10">
-        <f t="shared" ca="1" si="0"/>
-        <v>22000</v>
+        <f t="shared" si="0"/>
+        <v>21290.280000000006</v>
       </c>
       <c r="E23" s="8"/>
       <c r="F23" s="4"/>
@@ -2576,19 +2600,20 @@
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1">
       <c r="A24" s="7">
-        <f ca="1">EOMONTH(TODAY(),-1)+23</f>
-        <v>45253</v>
+        <f t="shared" si="2"/>
+        <v>45283</v>
       </c>
       <c r="B24" s="8">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C24" s="9">
-        <f ca="1">Info!D3-B24</f>
-        <v>1000</v>
+        <f>Info!D3-B24</f>
+        <v>967.74</v>
       </c>
       <c r="D24" s="10">
-        <f t="shared" ca="1" si="0"/>
-        <v>23000</v>
+        <f t="shared" si="0"/>
+        <v>22258.020000000008</v>
       </c>
       <c r="E24" s="8"/>
       <c r="F24" s="4"/>
@@ -2615,19 +2640,20 @@
     </row>
     <row r="25" spans="1:26" ht="15.75" customHeight="1">
       <c r="A25" s="7">
-        <f ca="1">EOMONTH(TODAY(),-1)+24</f>
-        <v>45254</v>
+        <f t="shared" si="2"/>
+        <v>45284</v>
       </c>
       <c r="B25" s="8">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C25" s="9">
-        <f ca="1">Info!D3-B25</f>
-        <v>1000</v>
+        <f>Info!D3-B25</f>
+        <v>967.74</v>
       </c>
       <c r="D25" s="10">
-        <f t="shared" ca="1" si="0"/>
-        <v>24000</v>
+        <f t="shared" si="0"/>
+        <v>23225.760000000009</v>
       </c>
       <c r="E25" s="8"/>
       <c r="F25" s="4"/>
@@ -2654,19 +2680,20 @@
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1">
       <c r="A26" s="7">
-        <f ca="1">EOMONTH(TODAY(),-1)+25</f>
-        <v>45255</v>
+        <f t="shared" si="2"/>
+        <v>45285</v>
       </c>
       <c r="B26" s="8">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C26" s="9">
-        <f ca="1">Info!D3-B26</f>
-        <v>1000</v>
+        <f>Info!D3-B26</f>
+        <v>967.74</v>
       </c>
       <c r="D26" s="10">
-        <f t="shared" ca="1" si="0"/>
-        <v>25000</v>
+        <f t="shared" si="0"/>
+        <v>24193.500000000011</v>
       </c>
       <c r="E26" s="8"/>
       <c r="F26" s="4"/>
@@ -2693,19 +2720,20 @@
     </row>
     <row r="27" spans="1:26" ht="15.75" customHeight="1">
       <c r="A27" s="7">
-        <f ca="1">EOMONTH(TODAY(),-1)+26</f>
-        <v>45256</v>
+        <f t="shared" si="2"/>
+        <v>45286</v>
       </c>
       <c r="B27" s="8">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C27" s="9">
-        <f ca="1">Info!D3-B27</f>
-        <v>1000</v>
+        <f>Info!D3-B27</f>
+        <v>967.74</v>
       </c>
       <c r="D27" s="10">
-        <f t="shared" ca="1" si="0"/>
-        <v>26000</v>
+        <f t="shared" si="0"/>
+        <v>25161.240000000013</v>
       </c>
       <c r="E27" s="8"/>
       <c r="F27" s="4"/>
@@ -2732,19 +2760,20 @@
     </row>
     <row r="28" spans="1:26" ht="15.75" customHeight="1">
       <c r="A28" s="7">
-        <f ca="1">EOMONTH(TODAY(),-1)+27</f>
-        <v>45257</v>
+        <f t="shared" si="2"/>
+        <v>45287</v>
       </c>
       <c r="B28" s="8">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C28" s="9">
-        <f ca="1">Info!D3-B28</f>
-        <v>1000</v>
+        <f>Info!D3-B28</f>
+        <v>967.74</v>
       </c>
       <c r="D28" s="10">
-        <f t="shared" ca="1" si="0"/>
-        <v>27000</v>
+        <f t="shared" si="0"/>
+        <v>26128.980000000014</v>
       </c>
       <c r="E28" s="8"/>
       <c r="F28" s="4"/>
@@ -2771,19 +2800,20 @@
     </row>
     <row r="29" spans="1:26" ht="15.75" customHeight="1">
       <c r="A29" s="7">
-        <f ca="1">EOMONTH(TODAY(),-1)+28</f>
-        <v>45258</v>
+        <f t="shared" si="2"/>
+        <v>45288</v>
       </c>
       <c r="B29" s="8">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C29" s="9">
-        <f ca="1">Info!D3-B29</f>
-        <v>1000</v>
+        <f>Info!D3-B29</f>
+        <v>967.74</v>
       </c>
       <c r="D29" s="10">
-        <f t="shared" ca="1" si="0"/>
-        <v>28000</v>
+        <f t="shared" si="0"/>
+        <v>27096.720000000016</v>
       </c>
       <c r="E29" s="8"/>
       <c r="F29" s="4"/>
@@ -2810,19 +2840,20 @@
     </row>
     <row r="30" spans="1:26" ht="15.75" customHeight="1">
       <c r="A30" s="7">
-        <f ca="1">EOMONTH(TODAY(),-1)+29</f>
-        <v>45259</v>
+        <f t="shared" si="2"/>
+        <v>45289</v>
       </c>
       <c r="B30" s="8">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C30" s="9">
-        <f ca="1">Info!D3-B30</f>
-        <v>1000</v>
+        <f>Info!D3-B30</f>
+        <v>967.74</v>
       </c>
       <c r="D30" s="10">
-        <f t="shared" ca="1" si="0"/>
-        <v>29000</v>
+        <f t="shared" si="0"/>
+        <v>28064.460000000017</v>
       </c>
       <c r="E30" s="8"/>
       <c r="F30" s="4"/>
@@ -2849,19 +2880,20 @@
     </row>
     <row r="31" spans="1:26" ht="15.75" customHeight="1">
       <c r="A31" s="7">
-        <f ca="1">EOMONTH(TODAY(),-1)+30</f>
-        <v>45260</v>
+        <f t="shared" si="2"/>
+        <v>45290</v>
       </c>
       <c r="B31" s="8">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C31" s="9">
-        <f ca="1">Info!D3-B31</f>
-        <v>1000</v>
+        <f>Info!D3-B31</f>
+        <v>967.74</v>
       </c>
       <c r="D31" s="10">
-        <f t="shared" ca="1" si="0"/>
-        <v>30000</v>
+        <f t="shared" si="0"/>
+        <v>29032.200000000019</v>
       </c>
       <c r="E31" s="8"/>
       <c r="F31" s="4"/>
@@ -2888,10 +2920,11 @@
     </row>
     <row r="32" spans="1:26" ht="15.75" customHeight="1">
       <c r="A32" s="7">
-        <f ca="1">EOMONTH(TODAY(),-1)+31</f>
-        <v>45261</v>
+        <f t="shared" si="2"/>
+        <v>45291</v>
       </c>
       <c r="B32" s="8">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C32" s="9">
@@ -2899,8 +2932,8 @@
         <v>0</v>
       </c>
       <c r="D32" s="10">
-        <f t="shared" ref="D32" ca="1" si="1">D31+C32</f>
-        <v>30000</v>
+        <f t="shared" ref="D32" si="3">D31+C32</f>
+        <v>29032.200000000019</v>
       </c>
       <c r="E32" s="8"/>
       <c r="F32" s="4"/>
@@ -30002,7 +30035,7 @@
       <c r="Z999" s="4"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="I2:I3 I35:I999 D1:D32">
+  <conditionalFormatting sqref="D1:D32 I2:I3 I35:I999">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThanOrEqual">
       <formula>1</formula>
     </cfRule>

</xml_diff>